<commit_message>
learning about exception handling in python
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Belajar\udemy\Data analyst Bootcamp\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{646BBAFF-8D93-4144-B286-100FB6B927AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E7705E-0A54-4E81-A689-A4DF2E82233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0FCC827-97E3-4E98-9870-BE76B2B14A0C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>jam</t>
   </si>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t xml:space="preserve">persentase </t>
+  </si>
+  <si>
+    <t>waktu hidup selama seminggu</t>
+  </si>
+  <si>
+    <t>waktu untuk bekerja selama seminggu</t>
+  </si>
+  <si>
+    <t>waktu tidur</t>
+  </si>
+  <si>
+    <t>waktu kuliah</t>
+  </si>
+  <si>
+    <t>waktu olahraga per minggu</t>
+  </si>
+  <si>
+    <t>waktu sisa per hari</t>
+  </si>
+  <si>
+    <t>waktu sisa per minggu</t>
+  </si>
+  <si>
+    <t>average 7 hari</t>
   </si>
 </sst>
 </file>
@@ -394,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68710C65-73C7-4347-93B6-974C60C6A482}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +436,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -421,47 +448,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f>24*7</f>
+        <v>168</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <f>P4/7</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <f>J3-(SUM(J4:J7))</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f>8*7</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f>7*2.5</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7.75</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f>AVERAGE(A2:A7)</f>
+        <v>7.958333333333333</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -469,7 +547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8.1999999999999993</v>
       </c>
@@ -478,6 +556,472 @@
       </c>
       <c r="C9">
         <v>11.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
at this commit, I learning about a topic about Data Analysis with python. first thing i learn how to use numpy and pandas library. I also lean about data visualization with matplotlib and seaborn
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Belajar\udemy\Data analyst Bootcamp\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E7705E-0A54-4E81-A689-A4DF2E82233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2066EFE-73B1-4C25-AC82-6AA633A330AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0FCC827-97E3-4E98-9870-BE76B2B14A0C}"/>
   </bookViews>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68710C65-73C7-4347-93B6-974C60C6A482}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,23 +570,47 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8.5</v>
+      </c>
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11">
+        <v>13.9</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
       <c r="B12">
         <v>11</v>
       </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8.5</v>
+      </c>
       <c r="B13">
         <v>12</v>
       </c>
+      <c r="C13">
+        <v>16.600000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5.5</v>
+      </c>
       <c r="B14">
         <v>13</v>
+      </c>
+      <c r="C14">
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
leaning about multi threading and multi processing with littlebit usecase implementation of it.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Belajar\udemy\Data analyst Bootcamp\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2066EFE-73B1-4C25-AC82-6AA633A330AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67FE631-365C-418A-897B-730DB45EBDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0FCC827-97E3-4E98-9870-BE76B2B14A0C}"/>
   </bookViews>
@@ -73,6 +73,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +425,7 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,6 +542,10 @@
       <c r="J7">
         <v>7</v>
       </c>
+      <c r="N7">
+        <f>84/451</f>
+        <v>0.18625277161862527</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -554,7 +562,7 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>11.9</v>
       </c>
     </row>
@@ -565,7 +573,7 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>13.3</v>
       </c>
     </row>
@@ -576,7 +584,7 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>13.9</v>
       </c>
     </row>
@@ -587,7 +595,7 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>15</v>
       </c>
     </row>
@@ -598,7 +606,7 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -609,96 +617,121 @@
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>17.100000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
       <c r="B15">
         <v>14</v>
       </c>
+      <c r="C15" s="1">
+        <f>82/451*100</f>
+        <v>18.181818181818183</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7</v>
+      </c>
       <c r="B16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6.5</v>
+      </c>
       <c r="B17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>8</v>
+      </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Learning about memory management in python
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Belajar\udemy\Data analyst Bootcamp\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67FE631-365C-418A-897B-730DB45EBDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02856DEF-E40B-40F3-ACA2-D926638A6CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0FCC827-97E3-4E98-9870-BE76B2B14A0C}"/>
   </bookViews>
@@ -105,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +426,13 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -451,6 +455,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="E2" s="2">
+        <v>45869</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -459,6 +466,9 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="E3" s="2">
+        <v>45870</v>
+      </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
@@ -481,6 +491,9 @@
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="E4" s="2">
+        <v>45871</v>
+      </c>
       <c r="F4" t="s">
         <v>4</v>
       </c>
@@ -502,6 +515,9 @@
       <c r="B5">
         <v>4</v>
       </c>
+      <c r="E5" s="2">
+        <v>45872</v>
+      </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
@@ -517,6 +533,9 @@
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="E6" s="2">
+        <v>45873</v>
+      </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
@@ -536,6 +555,9 @@
         <f>AVERAGE(A2:A7)</f>
         <v>7.958333333333333</v>
       </c>
+      <c r="E7" s="2">
+        <v>45874</v>
+      </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
@@ -554,6 +576,13 @@
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D19" si="0">AVERAGE(A3:A8)</f>
+        <v>6.958333333333333</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45875</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -565,6 +594,13 @@
       <c r="C9" s="1">
         <v>11.9</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7.3250000000000002</v>
+      </c>
+      <c r="E9" s="2">
+        <v>45876</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -576,6 +612,13 @@
       <c r="C10" s="1">
         <v>13.3</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>6.9916666666666671</v>
+      </c>
+      <c r="E10" s="2">
+        <v>45877</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -587,6 +630,13 @@
       <c r="C11" s="1">
         <v>13.9</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>7.0750000000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45878</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -598,6 +648,13 @@
       <c r="C12" s="1">
         <v>15</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6.9083333333333341</v>
+      </c>
+      <c r="E12" s="2">
+        <v>45879</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -609,6 +666,17 @@
       <c r="C13" s="1">
         <v>16.600000000000001</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>7.0333333333333341</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45880</v>
+      </c>
+      <c r="G13">
+        <f>94/451</f>
+        <v>0.20842572062084258</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -620,6 +688,13 @@
       <c r="C14" s="1">
         <v>17.100000000000001</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>7.2833333333333341</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45881</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -632,6 +707,13 @@
         <f>82/451*100</f>
         <v>18.181818181818183</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>7.083333333333333</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45882</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -643,8 +725,15 @@
       <c r="C16" s="1">
         <v>18.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6.916666666666667</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6.5</v>
       </c>
@@ -654,8 +743,15 @@
       <c r="C17" s="1">
         <v>18.600000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>6.583333333333333</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45884</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -665,73 +761,94 @@
       <c r="C18" s="1">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>7.083333333333333</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45885</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
       <c r="B19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Learning about flask framework
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Belajar\udemy\Data analyst Bootcamp\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02856DEF-E40B-40F3-ACA2-D926638A6CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44BD34E-7C72-4623-A6A3-63CE565D25FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0FCC827-97E3-4E98-9870-BE76B2B14A0C}"/>
   </bookViews>
@@ -423,18 +423,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68710C65-73C7-4347-93B6-974C60C6A482}">
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -458,8 +459,9 @@
       <c r="E2" s="2">
         <v>45869</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -469,22 +471,23 @@
       <c r="E3" s="2">
         <v>45870</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <f>24*7</f>
         <v>168</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>8</v>
       </c>
-      <c r="P3">
-        <f>P4/7</f>
+      <c r="R3">
+        <f>R4/7</f>
         <v>4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -494,21 +497,22 @@
       <c r="E4" s="2">
         <v>45871</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>56</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>9</v>
       </c>
-      <c r="P4">
-        <f>J3-(SUM(J4:J7))</f>
+      <c r="R4">
+        <f>L3-(SUM(L4:L7))</f>
         <v>31.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -518,15 +522,16 @@
       <c r="E5" s="2">
         <v>45872</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <f>8*7</f>
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -536,15 +541,16 @@
       <c r="E6" s="2">
         <v>45873</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <f>7*2.5</f>
         <v>17.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7.75</v>
       </c>
@@ -558,18 +564,19 @@
       <c r="E7" s="2">
         <v>45874</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>7</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <f>84/451</f>
         <v>0.18625277161862527</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -577,14 +584,15 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D19" si="0">AVERAGE(A3:A8)</f>
+        <f t="shared" ref="D8:D20" si="0">AVERAGE(A3:A8)</f>
         <v>6.958333333333333</v>
       </c>
       <c r="E8" s="2">
         <v>45875</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8.1999999999999993</v>
       </c>
@@ -601,8 +609,9 @@
       <c r="E9" s="2">
         <v>45876</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -619,8 +628,9 @@
       <c r="E10" s="2">
         <v>45877</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8.5</v>
       </c>
@@ -637,8 +647,9 @@
       <c r="E11" s="2">
         <v>45878</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -655,8 +666,13 @@
       <c r="E12" s="2">
         <v>45879</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+      <c r="H12">
+        <f>99/451</f>
+        <v>0.21951219512195122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8.5</v>
       </c>
@@ -673,12 +689,9 @@
       <c r="E13" s="2">
         <v>45880</v>
       </c>
-      <c r="G13">
-        <f>94/451</f>
-        <v>0.20842572062084258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5.5</v>
       </c>
@@ -695,8 +708,9 @@
       <c r="E14" s="2">
         <v>45881</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -714,8 +728,9 @@
       <c r="E15" s="2">
         <v>45882</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -732,8 +747,9 @@
       <c r="E16" s="2">
         <v>45883</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6.5</v>
       </c>
@@ -750,8 +766,9 @@
       <c r="E17" s="2">
         <v>45884</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -768,8 +785,9 @@
       <c r="E18" s="2">
         <v>45885</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7</v>
       </c>
@@ -786,69 +804,83 @@
       <c r="E19" s="2">
         <v>45886</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6.5</v>
+      </c>
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
+        <v>21.9</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE(A15:A20)</f>
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45887</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>31</v>
       </c>

</xml_diff>